<commit_message>
Completed all scripts with smoke test cases
</commit_message>
<xml_diff>
--- a/TestData/UBA_Portal_Login.xlsx
+++ b/TestData/UBA_Portal_Login.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Test_SetUP" sheetId="7" state="hidden" r:id="rId1"/>
     <sheet name="UBA_Login" sheetId="43" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="44" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="32">
   <si>
     <t>Environment</t>
   </si>
@@ -95,13 +96,22 @@
     <t>https://uba.adrl.in/auth/login</t>
   </si>
   <si>
+    <t>anshul@bizense.com</t>
+  </si>
+  <si>
+    <t>4850fgDjhWzZfE41N7rrig==</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>https://ubacpaas.terragonltd.com/auth/login</t>
+  </si>
+  <si>
     <t>qabizensetest+admin@gmail.com</t>
   </si>
   <si>
     <t>/ApO+Q68X+0WWy1v5QCRFg==</t>
-  </si>
-  <si>
-    <t>Production</t>
   </si>
 </sst>
 </file>
@@ -109,11 +119,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -124,18 +134,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -148,8 +146,110 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,14 +263,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -180,109 +272,27 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -305,181 +315,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,11 +518,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -528,6 +544,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -549,33 +574,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -597,10 +600,17 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -608,143 +618,143 @@
   </borders>
   <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -753,9 +763,9 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -766,13 +776,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="52" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="52" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="52" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="53">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1143,184 +1156,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" ht="14" spans="1:30">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="8">
         <v>1</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="AA2" s="8" t="s">
+      <c r="F2" s="7"/>
+      <c r="AA2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AB2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AC2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AD2" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" ht="14" spans="1:30">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="8">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="AA3" s="8" t="s">
+      <c r="F3" s="7"/>
+      <c r="AA3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="9" t="s">
+      <c r="AB3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
     </row>
     <row r="4" ht="14" spans="1:30">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="8">
         <v>1</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="AA4" s="8" t="s">
+      <c r="F4" s="7"/>
+      <c r="AA4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AB4" s="9" t="s">
+      <c r="AB4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AC4" s="9" t="s">
+      <c r="AC4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AD4" s="6" t="s">
+      <c r="AD4" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" ht="14" spans="1:27">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="8">
         <v>1</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="AA5" s="10"/>
+      <c r="F5" s="7"/>
+      <c r="AA5" s="11"/>
     </row>
     <row r="6" ht="14" spans="1:27">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="8">
         <v>1</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="AA6" s="10"/>
+      <c r="F6" s="7"/>
+      <c r="AA6" s="11"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="8">
         <v>1</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="8">
         <v>1</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -1354,7 +1367,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -1391,7 +1404,7 @@
       <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1403,9 +1416,15 @@
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:5">
@@ -1421,14 +1440,127 @@
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="E5" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="anshul@bizense.com"/>
+    <hyperlink ref="C5" r:id="rId1" display="anshul@bizense.com"/>
+    <hyperlink ref="B5" r:id="rId2" display="https://ubacpaas.terragonltd.com/auth/login"/>
+    <hyperlink ref="C2" r:id="rId1" display="anshul@bizense.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="13.2142857142857" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5714285714286" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.0714285714286" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7142857142857" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.64285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:5">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:5">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:5">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:5">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="anshul@bizense.com"/>
+    <hyperlink ref="C5" r:id="rId1" display="anshul@bizense.com"/>
+    <hyperlink ref="B5" r:id="rId2" display="https://ubacpaas.terragonltd.com/auth/login"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>